<commit_message>
fixing testing in K-folds
</commit_message>
<xml_diff>
--- a/QA_results.xlsx
+++ b/QA_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ml_learning\question_and_answer_task\Q_QA_task_original_code\quranqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB9D8A0-4A8D-45F4-9D99-61B749762C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E497AB-ACCF-4E1D-B421-5FF8A5A13F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,10 +316,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$I$2:$I$10</c:f>
+              <c:f>Tabelle1!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.56363196010244498</c:v>
                 </c:pt>
@@ -343,9 +343,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.50221992049707698</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.61142195150810297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,10 +382,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$J$2:$J$10</c:f>
+              <c:f>Tabelle1!$J$2:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.293577981651376</c:v>
                 </c:pt>
@@ -412,9 +409,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.247706422018348</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.302752293577981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,10 +448,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$K$2:$K$10</c:f>
+              <c:f>Tabelle1!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.53827443089773996</c:v>
                 </c:pt>
@@ -481,9 +475,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.46619978840787701</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.57376297124277398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2799,7 +2790,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I2" sqref="I2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>